<commit_message>
Changed resp_coeff spelling error
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_params_inputs_1col.xlsx
+++ b/notebooks/GenVeg/GenVeg_params_inputs_1col.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{183F660F-DA64-4AA7-BCEB-4ED58B5D2382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FAD9D3-1DD4-4FF9-96E7-CBDB274EAEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BTS" sheetId="4" r:id="rId1"/>
@@ -276,9 +276,6 @@
   </si>
   <si>
     <t>senescence_start</t>
-  </si>
-  <si>
-    <t>respiration_coeffecient</t>
   </si>
   <si>
     <t>glucose_requirement</t>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t>perennial</t>
+  </si>
+  <si>
+    <t>respiration_coefficient</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,14 +1078,14 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1093,14 +1093,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1108,14 +1108,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1123,14 +1123,14 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1141,11 +1141,11 @@
         <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1183,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="14">
@@ -1228,7 +1228,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>37</v>
@@ -1243,7 +1243,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>38</v>
@@ -1258,7 +1258,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>39</v>
@@ -1275,7 +1275,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>37</v>
@@ -1290,7 +1290,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>38</v>
@@ -1305,7 +1305,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>39</v>
@@ -1322,7 +1322,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="14">
@@ -1337,7 +1337,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="14">
@@ -1364,32 +1364,32 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="14"/>
       <c r="F23">
@@ -1399,10 +1399,10 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14"/>
       <c r="F24">
@@ -1412,10 +1412,10 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="14"/>
       <c r="F25">
@@ -1425,10 +1425,10 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="14"/>
       <c r="F26">
@@ -1438,10 +1438,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="D27" s="14"/>
       <c r="F27">
@@ -1453,7 +1453,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>37</v>
@@ -1468,7 +1468,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>38</v>
@@ -1483,7 +1483,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>39</v>
@@ -1512,7 +1512,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="14">
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="14">
@@ -1542,7 +1542,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="14">
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="14">
@@ -1572,7 +1572,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="14">
@@ -1584,7 +1584,7 @@
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="16"/>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="14">
@@ -1611,10 +1611,10 @@
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="14">
@@ -1626,10 +1626,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="14">
@@ -1656,7 +1656,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="14">
@@ -1671,7 +1671,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="14">
@@ -1698,7 +1698,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="14">
@@ -1716,7 +1716,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="14">
@@ -1745,7 +1745,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="21" t="s">
@@ -1763,7 +1763,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="14">
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="18">
         <v>1</v>
@@ -1793,7 +1793,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="18">
         <v>2</v>
@@ -1808,7 +1808,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="18">
         <v>3</v>
@@ -1823,7 +1823,7 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="18">
         <v>4</v>
@@ -1836,7 +1836,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="18">
         <v>5</v>
@@ -1851,7 +1851,7 @@
         <v>23</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="18">
         <v>1</v>
@@ -1866,7 +1866,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="18">
         <v>2</v>
@@ -1881,7 +1881,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="18">
         <v>3</v>
@@ -1896,7 +1896,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="18">
         <v>4</v>
@@ -1909,7 +1909,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="18">
         <v>5</v>
@@ -1924,7 +1924,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="18">
         <v>1</v>
@@ -1939,7 +1939,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -1954,7 +1954,7 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="18">
         <v>3</v>
@@ -1969,7 +1969,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="18">
         <v>4</v>
@@ -1982,7 +1982,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="18">
         <v>5</v>
@@ -1997,7 +1997,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="21" t="s">
@@ -2012,7 +2012,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="14">
@@ -2027,7 +2027,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -2042,7 +2042,7 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68" s="18">
         <v>2</v>
@@ -2057,7 +2057,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69" s="18">
         <v>3</v>
@@ -2072,7 +2072,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="18">
         <v>4</v>
@@ -2087,7 +2087,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="18">
         <v>5</v>
@@ -2104,7 +2104,7 @@
         <v>24</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" s="18">
         <v>1</v>
@@ -2119,7 +2119,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -2134,7 +2134,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="18">
         <v>3</v>
@@ -2149,7 +2149,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="18">
         <v>4</v>
@@ -2164,7 +2164,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C76" s="18">
         <v>5</v>
@@ -2181,7 +2181,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C77" s="18">
         <v>1</v>
@@ -2196,7 +2196,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -2211,7 +2211,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" s="18">
         <v>3</v>
@@ -2226,7 +2226,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C80" s="18">
         <v>4</v>
@@ -2241,7 +2241,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" s="18">
         <v>5</v>
@@ -2955,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F163672-6573-4055-B88E-D40A438226C7}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,14 +3002,14 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3017,14 +3017,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3032,14 +3032,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3047,14 +3047,14 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -3065,11 +3065,11 @@
         <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -3107,7 +3107,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="14">
@@ -3152,7 +3152,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>37</v>
@@ -3167,7 +3167,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>38</v>
@@ -3182,7 +3182,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>39</v>
@@ -3199,7 +3199,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>37</v>
@@ -3214,7 +3214,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>38</v>
@@ -3229,7 +3229,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>39</v>
@@ -3246,7 +3246,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="14">
@@ -3261,7 +3261,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="14">
@@ -3288,32 +3288,32 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="14"/>
       <c r="F23">
@@ -3323,10 +3323,10 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14"/>
       <c r="F24">
@@ -3336,10 +3336,10 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="14"/>
       <c r="F25">
@@ -3349,10 +3349,10 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="14"/>
       <c r="F26">
@@ -3362,10 +3362,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="D27" s="14"/>
       <c r="F27">
@@ -3377,7 +3377,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>37</v>
@@ -3392,7 +3392,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>38</v>
@@ -3407,7 +3407,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>39</v>
@@ -3436,7 +3436,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="14">
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="14">
@@ -3466,7 +3466,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="14">
@@ -3481,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="14">
@@ -3496,7 +3496,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="14">
@@ -3508,7 +3508,7 @@
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="16"/>
@@ -3520,10 +3520,10 @@
     </row>
     <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="14">
@@ -3535,10 +3535,10 @@
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="14">
@@ -3550,10 +3550,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="14">
@@ -3580,7 +3580,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="14">
@@ -3595,7 +3595,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="14">
@@ -3622,7 +3622,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="14">
@@ -3640,7 +3640,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="14">
@@ -3669,7 +3669,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="21" t="s">
@@ -3687,7 +3687,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="14">
@@ -3702,7 +3702,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="18">
         <v>1</v>
@@ -3717,7 +3717,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="18">
         <v>2</v>
@@ -3732,7 +3732,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="18">
         <v>3</v>
@@ -3747,7 +3747,7 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="18">
         <v>4</v>
@@ -3760,7 +3760,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="18">
         <v>5</v>
@@ -3775,7 +3775,7 @@
         <v>23</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="18">
         <v>1</v>
@@ -3790,7 +3790,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="18">
         <v>2</v>
@@ -3805,7 +3805,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="18">
         <v>3</v>
@@ -3820,7 +3820,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="18">
         <v>4</v>
@@ -3833,7 +3833,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="18">
         <v>5</v>
@@ -3848,7 +3848,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="18">
         <v>1</v>
@@ -3863,7 +3863,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -3878,7 +3878,7 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="18">
         <v>3</v>
@@ -3893,7 +3893,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="18">
         <v>4</v>
@@ -3906,7 +3906,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="18">
         <v>5</v>
@@ -3921,7 +3921,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="21" t="s">
@@ -3936,7 +3936,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="14">
@@ -3951,7 +3951,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -3966,7 +3966,7 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68" s="18">
         <v>2</v>
@@ -3981,7 +3981,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69" s="18">
         <v>3</v>
@@ -3996,7 +3996,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="18">
         <v>4</v>
@@ -4011,7 +4011,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="18">
         <v>5</v>
@@ -4028,7 +4028,7 @@
         <v>24</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" s="18">
         <v>1</v>
@@ -4043,7 +4043,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -4058,7 +4058,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="18">
         <v>3</v>
@@ -4073,7 +4073,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="18">
         <v>4</v>
@@ -4088,7 +4088,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C76" s="18">
         <v>5</v>
@@ -4105,7 +4105,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C77" s="18">
         <v>1</v>
@@ -4120,7 +4120,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -4135,7 +4135,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" s="18">
         <v>3</v>
@@ -4150,7 +4150,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C80" s="18">
         <v>4</v>
@@ -4165,7 +4165,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" s="18">
         <v>5</v>
@@ -4816,6 +4816,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4823,8 +4824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,14 +4871,14 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -4885,14 +4886,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -4900,14 +4901,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -4915,14 +4916,14 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -4933,11 +4934,11 @@
         <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -4975,7 +4976,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="14">
@@ -5020,7 +5021,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>37</v>
@@ -5035,7 +5036,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>38</v>
@@ -5050,7 +5051,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>39</v>
@@ -5067,7 +5068,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>37</v>
@@ -5082,7 +5083,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>38</v>
@@ -5097,7 +5098,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>39</v>
@@ -5114,7 +5115,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="14">
@@ -5129,7 +5130,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="14">
@@ -5156,32 +5157,32 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="14"/>
       <c r="F23">
@@ -5191,10 +5192,10 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14"/>
       <c r="F24">
@@ -5204,10 +5205,10 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="14"/>
       <c r="F25">
@@ -5217,10 +5218,10 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="14"/>
       <c r="F26">
@@ -5230,10 +5231,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="D27" s="14"/>
       <c r="F27">
@@ -5245,7 +5246,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>37</v>
@@ -5260,7 +5261,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>38</v>
@@ -5275,7 +5276,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>39</v>
@@ -5304,7 +5305,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="14">
@@ -5319,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="14">
@@ -5334,7 +5335,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="14">
@@ -5349,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="14">
@@ -5364,7 +5365,7 @@
         <v>46</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="14">
@@ -5376,7 +5377,7 @@
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="16"/>
@@ -5388,10 +5389,10 @@
     </row>
     <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="14">
@@ -5403,10 +5404,10 @@
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="14">
@@ -5418,10 +5419,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="14">
@@ -5448,7 +5449,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="14">
@@ -5463,7 +5464,7 @@
         <v>27</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="14">
@@ -5490,7 +5491,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="14">
@@ -5508,7 +5509,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="14">
@@ -5537,7 +5538,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="21" t="s">
@@ -5555,7 +5556,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="14">
@@ -5570,7 +5571,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="18">
         <v>1</v>
@@ -5585,7 +5586,7 @@
     <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="18">
         <v>2</v>
@@ -5600,7 +5601,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="18">
         <v>3</v>
@@ -5615,7 +5616,7 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="18">
         <v>4</v>
@@ -5628,7 +5629,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="18">
         <v>5</v>
@@ -5643,7 +5644,7 @@
         <v>23</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="18">
         <v>1</v>
@@ -5658,7 +5659,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="18">
         <v>2</v>
@@ -5673,7 +5674,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="18">
         <v>3</v>
@@ -5688,7 +5689,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C58" s="18">
         <v>4</v>
@@ -5701,7 +5702,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="18">
         <v>5</v>
@@ -5716,7 +5717,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="18">
         <v>1</v>
@@ -5731,7 +5732,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -5746,7 +5747,7 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="18">
         <v>3</v>
@@ -5761,7 +5762,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="18">
         <v>4</v>
@@ -5774,7 +5775,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="18">
         <v>5</v>
@@ -5789,7 +5790,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="21" t="s">
@@ -5804,7 +5805,7 @@
         <v>14</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="14">
@@ -5819,7 +5820,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -5834,7 +5835,7 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68" s="18">
         <v>2</v>
@@ -5849,7 +5850,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C69" s="18">
         <v>3</v>
@@ -5864,7 +5865,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" s="18">
         <v>4</v>
@@ -5879,7 +5880,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" s="18">
         <v>5</v>
@@ -5896,7 +5897,7 @@
         <v>24</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" s="18">
         <v>1</v>
@@ -5911,7 +5912,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -5926,7 +5927,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="18">
         <v>3</v>
@@ -5941,7 +5942,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="18">
         <v>4</v>
@@ -5956,7 +5957,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C76" s="18">
         <v>5</v>
@@ -5973,7 +5974,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C77" s="18">
         <v>1</v>
@@ -5988,7 +5989,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -6003,7 +6004,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" s="18">
         <v>3</v>
@@ -6018,7 +6019,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C80" s="18">
         <v>4</v>
@@ -6033,7 +6034,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81" s="18">
         <v>5</v>

</xml_diff>